<commit_message>
12 July Class Work Notes
</commit_message>
<xml_diff>
--- a/Fundamentals of statsitics (Bhumika Mam)/Block -II Central Tendency/Fundamentals Of Statistics  Block -II Central Tendency.xlsx
+++ b/Fundamentals of statsitics (Bhumika Mam)/Block -II Central Tendency/Fundamentals Of Statistics  Block -II Central Tendency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achyut Sharma\Documents\Data Sem 5\Fundamentals of statsitics (Bhumika Mam)\Block -II Central Tendency\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93443A75-FC10-4772-978C-A382A89BC869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E2673D-5855-458C-9F9E-734B9E8F2173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5 July 23" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="7 July 23(Q.4)" sheetId="5" r:id="rId5"/>
     <sheet name="10 July 23(class Practice)" sheetId="6" r:id="rId6"/>
     <sheet name="11 July 23(Class Practice)" sheetId="7" r:id="rId7"/>
+    <sheet name="12 July (C.P)" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="135">
   <si>
     <t>x</t>
   </si>
@@ -388,13 +389,216 @@
   </si>
   <si>
     <t>Second model or rule is that highest frequency is the mode as here 65 in above data.</t>
+  </si>
+  <si>
+    <t>find the mode in continous series</t>
+  </si>
+  <si>
+    <t>hightest frequency is 74 so 40--50 is z class</t>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">z is equal to </t>
+  </si>
+  <si>
+    <r>
+      <t>L+((F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/2F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*C)</t>
+    </r>
+  </si>
+  <si>
+    <t>Mode (Z) is equal to</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>as here f2 is not available so this binomial data we will use  z equal to 3M-2X(Bar) formula.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sigma(fx) </t>
+  </si>
+  <si>
+    <t>sigma(x)</t>
+  </si>
+  <si>
+    <t>M Class</t>
+  </si>
+  <si>
+    <t>(N/2)TH Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M CLASS </t>
+  </si>
+  <si>
+    <t>400-500</t>
+  </si>
+  <si>
+    <t>L+(((N/2)-CF/F)*C)</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>mean Or X(Bar)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +616,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1893,7 +2105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C562E4B3-F1DD-4D54-9228-88721399A648}">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
@@ -2574,8 +2786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E725250-D1B6-4147-9F28-BA6713235ED9}">
   <dimension ref="B3:N130"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="H125" sqref="H125"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2806,7 +3018,7 @@
     </row>
     <row r="36" spans="7:10" x14ac:dyDescent="0.3">
       <c r="J36">
-        <f>(E32/2)</f>
+        <f>E32/2</f>
         <v>19.5</v>
       </c>
     </row>
@@ -2904,7 +3116,7 @@
       </c>
     </row>
     <row r="68" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C68" s="4" t="s">
+      <c r="C68" t="s">
         <v>102</v>
       </c>
       <c r="D68">
@@ -3151,6 +3363,347 @@
     <row r="130" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C130" t="s">
         <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A086EF-2B12-46F7-914E-304174CC141F}">
+  <dimension ref="C3:M52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="2">
+        <v>74</v>
+      </c>
+      <c r="E12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="F18" t="s">
+        <v>121</v>
+      </c>
+      <c r="H18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <f>(D12-D11)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <f>(2*D12)-D11-D13</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <f>H19/H20</f>
+        <v>0.21052631578947367</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <f>H21*10</f>
+        <v>2.1052631578947367</v>
+      </c>
+    </row>
+    <row r="23" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>123</v>
+      </c>
+      <c r="H23" s="2">
+        <f>40+H22</f>
+        <v>42.10526315789474</v>
+      </c>
+    </row>
+    <row r="33" spans="4:13" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="E33" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36">
+        <v>15</v>
+      </c>
+      <c r="F36">
+        <v>150</v>
+      </c>
+      <c r="G36">
+        <f>F36*E36</f>
+        <v>2250</v>
+      </c>
+      <c r="H36">
+        <f>15</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37">
+        <v>33</v>
+      </c>
+      <c r="F37">
+        <v>250</v>
+      </c>
+      <c r="G37">
+        <f t="shared" ref="G37:G40" si="0">F37*E37</f>
+        <v>8250</v>
+      </c>
+      <c r="H37">
+        <f>H36+E37</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38">
+        <v>63</v>
+      </c>
+      <c r="F38">
+        <v>350</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>22050</v>
+      </c>
+      <c r="H38">
+        <f t="shared" ref="H38:H40" si="1">H37+E38</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="4:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D39" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="2">
+        <v>85</v>
+      </c>
+      <c r="F39" s="2">
+        <v>450</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="0"/>
+        <v>38250</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="1"/>
+        <v>196</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="L39" s="2">
+        <f>AVERAGE(H41/E42)</f>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D40" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="4">
+        <v>100</v>
+      </c>
+      <c r="F40">
+        <v>550</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>55000</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>296</v>
+      </c>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="G41" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H41" s="2">
+        <f>SUM(G36:G40)</f>
+        <v>125800</v>
+      </c>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D42" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E42" s="2">
+        <f>SUM(E36:E40)</f>
+        <v>296</v>
+      </c>
+      <c r="K42" t="s">
+        <v>128</v>
+      </c>
+      <c r="L42" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="L43">
+        <f>H40/2</f>
+        <v>148</v>
+      </c>
+      <c r="M43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="K44" t="s">
+        <v>130</v>
+      </c>
+      <c r="L44" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="K47" t="s">
+        <v>61</v>
+      </c>
+      <c r="L47" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="L48">
+        <f>L43-111</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L49">
+        <f>L48/85</f>
+        <v>0.43529411764705883</v>
+      </c>
+    </row>
+    <row r="50" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="L50">
+        <f>L49*100</f>
+        <v>43.529411764705884</v>
+      </c>
+    </row>
+    <row r="51" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K51" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L51" s="2">
+        <f>L50+400</f>
+        <v>443.52941176470586</v>
+      </c>
+    </row>
+    <row r="52" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K52" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L52" s="2">
+        <f>(3*L51)-(2*L39)</f>
+        <v>480.58823529411757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>